<commit_message>
Add decirate Have buff
</commit_message>
<xml_diff>
--- a/Project/Tools/Excel/plan/excel/Common/TablePropItem.xlsx
+++ b/Project/Tools/Excel/plan/excel/Common/TablePropItem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\UnityProject\BagBattle\Project\Tools\Excel\plan\excel\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E81CA77-F2EC-4C02-B385-5757CD566FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C727AB1-CE80-44E5-865C-BE9C222424BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32355" yWindow="1380" windowWidth="25710" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24210" yWindow="1515" windowWidth="29010" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -708,7 +708,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -777,12 +777,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1853,7 +1847,7 @@
       <c r="M11" s="1">
         <v>-1</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="19" t="s">
         <v>98</v>
       </c>
       <c r="O11" s="19" t="s">
@@ -1918,7 +1912,7 @@
       <c r="M12" s="1">
         <v>-1</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="1">
         <v>3</v>
       </c>
       <c r="O12" s="1">
@@ -1983,7 +1977,7 @@
       <c r="M13" s="1">
         <v>-1</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="1">
         <v>3</v>
       </c>
       <c r="O13" s="19">
@@ -2048,7 +2042,7 @@
       <c r="M14" s="1">
         <v>-1</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="1">
         <v>6</v>
       </c>
       <c r="O14" s="19" t="s">

</xml_diff>